<commit_message>
performance tests for dslookup are added
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-tests/engine-it-performance/src/test/resources/dataset/ShuffledDataSet100.xlsx
+++ b/calculation-engine/engine-tests/engine-it-performance/src/test/resources/dataset/ShuffledDataSet100.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="28800" windowHeight="12570"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="28800" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="ShuffledDataSet100" sheetId="1" r:id="rId1"/>
@@ -973,7 +973,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>